<commit_message>
data entry + ind button
gems added
individual treasure loot tables added
started ind tres button execution
</commit_message>
<xml_diff>
--- a/Items/Loot_Formatting.xlsx
+++ b/Items/Loot_Formatting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon.withrow\Dropbox\Home-Work Share\DnD_Loot_Gen\GitHub\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65D80F3-39E0-43AB-95C8-672C080DC588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBBE9CF-A820-425F-9D29-1C0B2F4D29B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{D978C551-18DF-42F1-ADFB-F930610F9EF0}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="12" xr2:uid="{D978C551-18DF-42F1-ADFB-F930610F9EF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_Weapons" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,11 @@
     <sheet name="Basic_Armor" sheetId="13" r:id="rId10"/>
     <sheet name="Magic_Armor" sheetId="11" r:id="rId11"/>
     <sheet name="Shield" sheetId="14" r:id="rId12"/>
+    <sheet name="GEMS" sheetId="15" r:id="rId13"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">GEMS!$B$1:$C$127</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3395" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="774">
   <si>
     <t>Rarity</t>
   </si>
@@ -1947,9 +1951,6 @@
     <t>Shield of Missile Attraction</t>
   </si>
   <si>
-    <t>Shield, +2</t>
-  </si>
-  <si>
     <t>Adamantine Armor</t>
   </si>
   <si>
@@ -1962,9 +1963,6 @@
     <t>Sentinel Shield</t>
   </si>
   <si>
-    <t>Shield, +1</t>
-  </si>
-  <si>
     <t>Animated Shield</t>
   </si>
   <si>
@@ -1980,9 +1978,6 @@
     <t>Dwarven Plate</t>
   </si>
   <si>
-    <t>Shield, +3</t>
-  </si>
-  <si>
     <t>Spellguard Shield</t>
   </si>
   <si>
@@ -1992,9 +1987,6 @@
     <t>Plate</t>
   </si>
   <si>
-    <t>Light:Medium:Heavy</t>
-  </si>
-  <si>
     <t>Shield</t>
   </si>
   <si>
@@ -2062,13 +2054,331 @@
   </si>
   <si>
     <t>Shield, +3 in addition</t>
+  </si>
+  <si>
+    <t>Gem</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>A transparent dark green gemstone</t>
+  </si>
+  <si>
+    <t>A transparent deep purple gemstone</t>
+  </si>
+  <si>
+    <t>A transparent pale blue-green gemstone</t>
+  </si>
+  <si>
+    <t>A transparent watery gold to rich gold gemstone</t>
+  </si>
+  <si>
+    <t>An opaque mottled deep blue gemstone</t>
+  </si>
+  <si>
+    <t>A translucent striped brown, blue, white, or red gemstone</t>
+  </si>
+  <si>
+    <t>A translucent dark green with black mottling and golden flecks gemstone</t>
+  </si>
+  <si>
+    <t>An opaque pure black gemstone</t>
+  </si>
+  <si>
+    <t>A translucent lustrous black gemstone with glowing highlights</t>
+  </si>
+  <si>
+    <t>An opaque dark gray gemstone with red flecks</t>
+  </si>
+  <si>
+    <t>A transparent pale blue gemstone</t>
+  </si>
+  <si>
+    <t>A transparent blue-white to medium blue gemstone</t>
+  </si>
+  <si>
+    <t>A transparent deep blue gemstone</t>
+  </si>
+  <si>
+    <t>An opaque orange to red-brown gemstone</t>
+  </si>
+  <si>
+    <t>An opaque white gemstone</t>
+  </si>
+  <si>
+    <t>A transparent yellow-green to pale green gemstone</t>
+  </si>
+  <si>
+    <t>A translucent green gemstone</t>
+  </si>
+  <si>
+    <t>A transparent pale yellow-brown gemstone</t>
+  </si>
+  <si>
+    <t>An opaque crimson gemstone</t>
+  </si>
+  <si>
+    <t>A transparent blue-white, canary, pink, brown, or blue gemstone</t>
+  </si>
+  <si>
+    <t>A transparent deep bright green gemstone</t>
+  </si>
+  <si>
+    <t>A translucent gemstone with circles of gray, white, brown, blue, or green</t>
+  </si>
+  <si>
+    <t>A translucent fiery red Gemstone</t>
+  </si>
+  <si>
+    <t>A transparent red, brown-green, or violet gemstone</t>
+  </si>
+  <si>
+    <t>An opaque gray-black gemstone</t>
+  </si>
+  <si>
+    <t>A transparent fiery orange gemstone</t>
+  </si>
+  <si>
+    <t>A translucent light green, deep green, or white gemstone</t>
+  </si>
+  <si>
+    <t>An opaque blue, black, or brown gemstone</t>
+  </si>
+  <si>
+    <t>An opaque deep black gemstone</t>
+  </si>
+  <si>
+    <t>An opaque light and dark blue gemstone with yellow flecks</t>
+  </si>
+  <si>
+    <t>An opaque striated light and dark green gemstone</t>
+  </si>
+  <si>
+    <t>A translucent white gemstone with a pale blue glow</t>
+  </si>
+  <si>
+    <t>A translucent gemstone with pink or yellow-white with mossy gray or green markings</t>
+  </si>
+  <si>
+    <t>An opaque black gemstone</t>
+  </si>
+  <si>
+    <t>An opaque gemstone with bands of black and white, or pure black or white</t>
+  </si>
+  <si>
+    <t>A translucent pale blue with green and golden mottling gemstone</t>
+  </si>
+  <si>
+    <t>An opaque lustrous white, yellow, or pink gemstone</t>
+  </si>
+  <si>
+    <t>A transparent rich olive green gemstone</t>
+  </si>
+  <si>
+    <t>A transparent white, smoky gray, or yellow gemstone</t>
+  </si>
+  <si>
+    <t>An opaque light pink gemstone</t>
+  </si>
+  <si>
+    <t>A transparent clear red to deep crimson gemstone</t>
+  </si>
+  <si>
+    <t>An opaque gemstone with bands of red and white</t>
+  </si>
+  <si>
+    <t>A transparent gemstone of red, red-brown, or deep green</t>
+  </si>
+  <si>
+    <t>A translucent rosy Gemstone with a white star-shaped center</t>
+  </si>
+  <si>
+    <t>A translucent ruby gemstone with a white star-shaped center</t>
+  </si>
+  <si>
+    <t>A translucent blue sapphire gemstone with a white star-shaped center</t>
+  </si>
+  <si>
+    <t>A translucent brown gemstone with a golden center</t>
+  </si>
+  <si>
+    <t>A transparent golden yellow gemstone</t>
+  </si>
+  <si>
+    <t>A transparent pale green, blue, brown, or red gemstone</t>
+  </si>
+  <si>
+    <t>An opaque light blue-green gemstone</t>
+  </si>
+  <si>
+    <t>A transparent fiery yellow or yellow-green gemstone</t>
+  </si>
+  <si>
+    <t>Azurite</t>
+  </si>
+  <si>
+    <t>Banded Agate</t>
+  </si>
+  <si>
+    <t>Blue quartz</t>
+  </si>
+  <si>
+    <t>Eye agate</t>
+  </si>
+  <si>
+    <t>Hematite</t>
+  </si>
+  <si>
+    <t>Lapis Lazuli</t>
+  </si>
+  <si>
+    <t>Malachite</t>
+  </si>
+  <si>
+    <t>Moss agate</t>
+  </si>
+  <si>
+    <t>Obsidian</t>
+  </si>
+  <si>
+    <t>Rhodochrosite</t>
+  </si>
+  <si>
+    <t>Tiger Eye</t>
+  </si>
+  <si>
+    <t>Turquoise</t>
+  </si>
+  <si>
+    <t>Bloodstone</t>
+  </si>
+  <si>
+    <t>Carnelian</t>
+  </si>
+  <si>
+    <t>Chalcedony</t>
+  </si>
+  <si>
+    <t>Chrysoprase</t>
+  </si>
+  <si>
+    <t>Citrine</t>
+  </si>
+  <si>
+    <t>Jasper</t>
+  </si>
+  <si>
+    <t>Moonstone</t>
+  </si>
+  <si>
+    <t>Onyx</t>
+  </si>
+  <si>
+    <t>Quartz</t>
+  </si>
+  <si>
+    <t>Sardonyx</t>
+  </si>
+  <si>
+    <t>Star Rose Quartz</t>
+  </si>
+  <si>
+    <t>Zircon</t>
+  </si>
+  <si>
+    <t>Amber</t>
+  </si>
+  <si>
+    <t>Amethyst</t>
+  </si>
+  <si>
+    <t>Chrysoberyl</t>
+  </si>
+  <si>
+    <t>Coral</t>
+  </si>
+  <si>
+    <t>Garnet</t>
+  </si>
+  <si>
+    <t>Jade</t>
+  </si>
+  <si>
+    <t>Jet</t>
+  </si>
+  <si>
+    <t>Pearl</t>
+  </si>
+  <si>
+    <t>Spinel</t>
+  </si>
+  <si>
+    <t>Tourmaline</t>
+  </si>
+  <si>
+    <t>Alexandrite</t>
+  </si>
+  <si>
+    <t>Aquamarine</t>
+  </si>
+  <si>
+    <t>Black Pearl</t>
+  </si>
+  <si>
+    <t>Blue spinel</t>
+  </si>
+  <si>
+    <t>Peridot</t>
+  </si>
+  <si>
+    <t>Topaz</t>
+  </si>
+  <si>
+    <t>Black Opal</t>
+  </si>
+  <si>
+    <t>Blue Sapphire</t>
+  </si>
+  <si>
+    <t>Emerald</t>
+  </si>
+  <si>
+    <t>Fire Opal</t>
+  </si>
+  <si>
+    <t>Opal</t>
+  </si>
+  <si>
+    <t>Star Ruby</t>
+  </si>
+  <si>
+    <t>Star Sapphire</t>
+  </si>
+  <si>
+    <t>Yellow sapphire</t>
+  </si>
+  <si>
+    <t>Black Sapphire</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>Jacinth</t>
+  </si>
+  <si>
+    <t>Ruby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2084,6 +2394,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2117,7 +2436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2143,6 +2462,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5159,7 +5485,7 @@
   <dimension ref="A1:M265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5206,13 +5532,13 @@
         <v>265</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>272</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
@@ -5228,7 +5554,7 @@
         <v>C;Body;N;[Basic_Armor];0;-;PHB(130)</v>
       </c>
       <c r="M2" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5236,13 +5562,13 @@
         <v>265</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>272</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -5254,11 +5580,11 @@
         <v>352</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I66" si="0">_xlfn.CONCAT(A3,";",B3,";",C3,";",D3,";",E3,";",F3,";",G3)</f>
+        <f t="shared" ref="I3:I24" si="0">_xlfn.CONCAT(A3,";",B3,";",C3,";",D3,";",E3,";",F3,";",G3)</f>
         <v>C;Head:Glove:Boot;N;[Basic_Armor];1;-;PHB(130)</v>
       </c>
       <c r="M3" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -5266,13 +5592,13 @@
         <v>266</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>272</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -5284,11 +5610,11 @@
         <v>352</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I16" si="1">_xlfn.CONCAT(A12,";",B12,";",C12,";",D12,";",E12,";",F12,";",G12)</f>
-        <v>;;;;;;</v>
+        <f t="shared" si="0"/>
+        <v>U;Body;N;[Basic_Armor];1;-;PHB(130)</v>
       </c>
       <c r="M4" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -5296,13 +5622,13 @@
         <v>266</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>272</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -5314,11 +5640,11 @@
         <v>352</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="1"/>
-        <v>V;Any;N;[Basic_Armor] +2;2;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>U;Amulet:Belt;N;[Basic_Armor];1;-;PHB(130)</v>
       </c>
       <c r="M5" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -5326,13 +5652,13 @@
         <v>266</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>272</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E6" s="3">
         <v>2</v>
@@ -5344,11 +5670,11 @@
         <v>352</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="1"/>
-        <v>V;Any;N;[Basic_Armor] +1;3;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>U;Head:Glove:Boot;N;[Basic_Armor];2;-;PHB(130)</v>
       </c>
       <c r="M6" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -5356,13 +5682,13 @@
         <v>267</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>272</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E7" s="3">
         <v>2</v>
@@ -5374,11 +5700,11 @@
         <v>352</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="1"/>
-        <v>R;Any;N;[Basic_Armor] +1;2;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>R;Body;N;[Basic_Armor];2;-;PHB(130)</v>
       </c>
       <c r="M7" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -5386,13 +5712,13 @@
         <v>267</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>272</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -5404,26 +5730,26 @@
         <v>352</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="1"/>
-        <v>R;Any;N;[Basic_Armor];3;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>R;Body;N;[Basic_Armor] +1;0;-;PHB(130)</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I9" t="str">
-        <f t="shared" si="1"/>
-        <v>V;Any;N;[Basic_Armor] +3;1;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>;;;;;;</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I10" t="str">
-        <f t="shared" si="1"/>
-        <v>V;Any;N;[Basic_Armor] +2;2;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>;;;;;;</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I11" t="str">
-        <f t="shared" si="1"/>
-        <v>V;Any;N;[Basic_Armor] +1;3;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>;;;;;;</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -5432,8 +5758,8 @@
       <c r="E12" s="3"/>
       <c r="F12" s="10"/>
       <c r="I12" t="str">
-        <f t="shared" si="1"/>
-        <v>V;Any;N;[Basic_Armor];4;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>;;;;;;</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -5447,7 +5773,7 @@
         <v>272</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="E13" s="3">
         <v>2</v>
@@ -5459,8 +5785,8 @@
         <v>352</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="1"/>
-        <v>L;Any;N;[Basic_Armor] +3;2;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>V;Any;N;[Basic_Armor] +2;2;-;PHB(130)</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -5474,7 +5800,7 @@
         <v>272</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E14" s="3">
         <v>3</v>
@@ -5486,8 +5812,8 @@
         <v>352</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="1"/>
-        <v>L;Any;N;[Basic_Armor] +2;3;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>V;Any;N;[Basic_Armor] +1;3;-;PHB(130)</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -5501,7 +5827,7 @@
         <v>272</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E15" s="3">
         <v>2</v>
@@ -5513,8 +5839,8 @@
         <v>352</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="1"/>
-        <v>L;Any;N;[Basic_Armor] +1;4;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>R;Any;N;[Basic_Armor] +1;2;-;PHB(130)</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -5528,7 +5854,7 @@
         <v>272</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E16" s="3">
         <v>3</v>
@@ -5540,8 +5866,8 @@
         <v>352</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="1"/>
-        <v>L;Any;N;[Basic_Armor];5;-;PHB(130)</v>
+        <f t="shared" si="0"/>
+        <v>R;Any;N;[Basic_Armor];3;-;PHB(130)</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -5555,7 +5881,7 @@
         <v>272</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -5566,9 +5892,9 @@
       <c r="G17" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I17" t="e">
-        <f>_xlfn.CONCAT(#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!)</f>
-        <v>#REF!</v>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>V;Any;N;[Basic_Armor] +3;1;-;PHB(130)</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -5582,7 +5908,7 @@
         <v>272</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="E18" s="3">
         <v>2</v>
@@ -5593,9 +5919,9 @@
       <c r="G18" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I18" t="e">
-        <f>_xlfn.CONCAT(#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!)</f>
-        <v>#REF!</v>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>V;Any;N;[Basic_Armor] +2;2;-;PHB(130)</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -5609,7 +5935,7 @@
         <v>272</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E19" s="3">
         <v>3</v>
@@ -5620,9 +5946,9 @@
       <c r="G19" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I19" t="e">
-        <f>_xlfn.CONCAT(#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!)</f>
-        <v>#REF!</v>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>V;Any;N;[Basic_Armor] +1;3;-;PHB(130)</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -5636,7 +5962,7 @@
         <v>272</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E20" s="3">
         <v>4</v>
@@ -5647,9 +5973,9 @@
       <c r="G20" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I20" t="e">
-        <f>_xlfn.CONCAT(#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!)</f>
-        <v>#REF!</v>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>V;Any;N;[Basic_Armor];4;-;PHB(130)</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -5663,7 +5989,7 @@
         <v>272</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="E21" s="3">
         <v>2</v>
@@ -5674,9 +6000,9 @@
       <c r="G21" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I21" t="e">
-        <f>_xlfn.CONCAT(#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!)</f>
-        <v>#REF!</v>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>L;Any;N;[Basic_Armor] +3;2;-;PHB(130)</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -5690,7 +6016,7 @@
         <v>272</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="E22" s="3">
         <v>3</v>
@@ -5701,9 +6027,9 @@
       <c r="G22" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I22" t="e">
-        <f>_xlfn.CONCAT(#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!)</f>
-        <v>#REF!</v>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>L;Any;N;[Basic_Armor] +2;3;-;PHB(130)</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -5717,7 +6043,7 @@
         <v>272</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="E23" s="3">
         <v>4</v>
@@ -5728,9 +6054,9 @@
       <c r="G23" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I23" t="e">
-        <f>_xlfn.CONCAT(#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!)</f>
-        <v>#REF!</v>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>L;Any;N;[Basic_Armor] +1;4;-;PHB(130)</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -5744,7 +6070,7 @@
         <v>272</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E24" s="3">
         <v>5</v>
@@ -5755,9 +6081,9 @@
       <c r="G24" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I24" t="e">
-        <f>_xlfn.CONCAT(#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!,";",#REF!)</f>
-        <v>#REF!</v>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>L;Any;N;[Basic_Armor];5;-;PHB(130)</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -5765,7 +6091,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="3"/>
       <c r="I25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I25:I66" si="1">_xlfn.CONCAT(A25,";",B25,";",C25,";",D25,";",E25,";",F25,";",G25)</f>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5774,7 +6100,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
       <c r="I26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5783,7 +6109,7 @@
       <c r="D27" s="4"/>
       <c r="E27" s="3"/>
       <c r="I27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5792,7 +6118,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="3"/>
       <c r="I28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5801,7 +6127,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="3"/>
       <c r="I29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5810,7 +6136,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="3"/>
       <c r="I30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5819,7 +6145,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="3"/>
       <c r="I31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5828,7 +6154,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="3"/>
       <c r="I32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5837,7 +6163,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="3"/>
       <c r="I33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5846,7 +6172,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="3"/>
       <c r="I34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5855,7 +6181,7 @@
       <c r="D35" s="4"/>
       <c r="E35" s="3"/>
       <c r="I35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5864,7 +6190,7 @@
       <c r="D36" s="4"/>
       <c r="E36" s="3"/>
       <c r="I36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5873,7 +6199,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
       <c r="I37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5882,7 +6208,7 @@
       <c r="D38" s="4"/>
       <c r="E38" s="3"/>
       <c r="I38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5891,7 +6217,7 @@
       <c r="D39" s="4"/>
       <c r="E39" s="3"/>
       <c r="I39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5900,7 +6226,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="3"/>
       <c r="I40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5909,7 +6235,7 @@
       <c r="D41" s="4"/>
       <c r="E41" s="3"/>
       <c r="I41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5918,7 +6244,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="3"/>
       <c r="I42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5927,7 +6253,7 @@
       <c r="D43" s="4"/>
       <c r="E43" s="3"/>
       <c r="I43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5936,7 +6262,7 @@
       <c r="D44" s="4"/>
       <c r="E44" s="3"/>
       <c r="I44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5945,7 +6271,7 @@
       <c r="D45" s="4"/>
       <c r="E45" s="3"/>
       <c r="I45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5954,7 +6280,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="3"/>
       <c r="I46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5963,7 +6289,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="3"/>
       <c r="I47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5972,7 +6298,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="3"/>
       <c r="I48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5981,7 +6307,7 @@
       <c r="D49" s="4"/>
       <c r="E49" s="3"/>
       <c r="I49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5990,7 +6316,7 @@
       <c r="D50" s="4"/>
       <c r="E50" s="3"/>
       <c r="I50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -5999,7 +6325,7 @@
       <c r="D51" s="4"/>
       <c r="E51" s="3"/>
       <c r="I51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6008,7 +6334,7 @@
       <c r="D52" s="4"/>
       <c r="E52" s="3"/>
       <c r="I52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6017,7 +6343,7 @@
       <c r="D53" s="4"/>
       <c r="E53" s="3"/>
       <c r="I53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6026,7 +6352,7 @@
       <c r="D54" s="4"/>
       <c r="E54" s="3"/>
       <c r="I54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6035,7 +6361,7 @@
       <c r="D55" s="4"/>
       <c r="E55" s="3"/>
       <c r="I55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6044,7 +6370,7 @@
       <c r="D56" s="4"/>
       <c r="E56" s="3"/>
       <c r="I56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6053,7 +6379,7 @@
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
       <c r="I57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6062,7 +6388,7 @@
       <c r="D58" s="4"/>
       <c r="E58" s="3"/>
       <c r="I58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6071,7 +6397,7 @@
       <c r="D59" s="4"/>
       <c r="E59" s="3"/>
       <c r="I59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6080,7 +6406,7 @@
       <c r="D60" s="4"/>
       <c r="E60" s="3"/>
       <c r="I60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6089,7 +6415,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="3"/>
       <c r="I61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6098,7 +6424,7 @@
       <c r="D62" s="4"/>
       <c r="E62" s="3"/>
       <c r="I62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6107,7 +6433,7 @@
       <c r="D63" s="4"/>
       <c r="E63" s="3"/>
       <c r="I63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6116,7 +6442,7 @@
       <c r="D64" s="4"/>
       <c r="E64" s="3"/>
       <c r="I64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6125,7 +6451,7 @@
       <c r="D65" s="4"/>
       <c r="E65" s="3"/>
       <c r="I65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -6134,7 +6460,7 @@
       <c r="D66" s="4"/>
       <c r="E66" s="3"/>
       <c r="I66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>;;;;;;</v>
       </c>
     </row>
@@ -7940,7 +8266,7 @@
   <dimension ref="A1:L265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="H1" activeCellId="1" sqref="G1:G1048576 H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7987,6 +8313,9 @@
       <c r="B2" s="3" t="s">
         <v>405</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="D2" s="4" t="s">
         <v>616</v>
       </c>
@@ -7998,7 +8327,7 @@
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(A2,";",B2,";",C2,";",D2,";",E2,";",F2)</f>
-        <v>C;Any;;Armor of Gleaming;-;XGE(136)</v>
+        <v>C;Any;N;Armor of Gleaming;-;XGE(136)</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>467</v>
@@ -8016,7 +8345,10 @@
         <v>265</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>648</v>
+        <v>405</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>617</v>
@@ -8029,7 +8361,7 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">CONCATENATE(A3,";",B3,";",C3,";",D3,";",E3,";",F3)</f>
-        <v>C;Light:Medium:Heavy;;Cast-Off Armor;-;XGE(136)</v>
+        <v>C;Any;N;Cast-Off Armor;-;XGE(136)</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>467</v>
@@ -8047,10 +8379,13 @@
         <v>265</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>649</v>
+        <v>405</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>476</v>
@@ -8060,7 +8395,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>C;Shield;;Shield of Expression;-;XGE(139)</v>
+        <v>C;Any;N;Smoldering Armor;-;XGE(139)</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>467</v>
@@ -8075,21 +8410,26 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>269</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D5" s="4" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>344</v>
+        <v>279</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>C;;;Smoldering Armor;-;XGE(139)</v>
+        <v>L;Plate;Y;Armor of Invulnerability;-;DMG(152)</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>467</v>
@@ -8107,13 +8447,13 @@
         <v>269</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>647</v>
+        <v>405</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>476</v>
@@ -8123,7 +8463,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>L;Plate;Y;Armor of Invulnerability;-;DMG(152)</v>
+        <v>L;Any;N;Armor, +3;-;DMG(152)</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>469</v>
@@ -8140,19 +8480,24 @@
       <c r="A7" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>279</v>
+        <v>300</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>L;;;Armor, +3;-;DMG(152)</v>
+        <v>L;Chain_Mail;Y;Efreeti Chain;-;DMG(167)</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>469</v>
@@ -8170,23 +8515,23 @@
         <v>269</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>273</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>L;Chain_Mail;Y;Efreeti Chain;-;DMG(167)</v>
+        <v>L;Plate;Y;Plate Armor of Etherealness;-;DMG(185)</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>469</v>
@@ -8201,26 +8546,26 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>476</v>
+        <v>650</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>L;Plate;Y;Plate Armor of Etherealness;-;DMG(185)</v>
+        <v>R;Medium:Heavy;N;Mizzium Armor;Not Hide;GGR(179)</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>469</v>
@@ -8237,19 +8582,24 @@
       <c r="A10" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D10" s="4" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>320</v>
+        <v>279</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>R;;;Mizzium Armor;-;GGR(179)</v>
+        <v>R;Any;Y;Armor of Resistance;-;DMG(152)</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>570</v>
@@ -8266,19 +8616,24 @@
       <c r="A11" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D11" s="4" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>325</v>
+        <v>279</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>R;;;Pariah's Shield;-;GGR(180)</v>
+        <v>R;Plate;Y;Armor of Vulnerability;-;DMG(152)</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>570</v>
@@ -8295,12 +8650,14 @@
       <c r="A12" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>405</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>476</v>
@@ -8310,7 +8667,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>R;;Y;Armor of Resistance;-;DMG(152)</v>
+        <v>R;Any;N;Armor, +1;-;DMG(152)</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>469</v>
@@ -8328,23 +8685,23 @@
         <v>267</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>R;Plate;Y;Armor of Vulnerability;-;DMG(152)</v>
+        <v>R;Chain_Shirt;N;Elven Chain;-;DMG(168)</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>469</v>
@@ -8361,19 +8718,24 @@
       <c r="A14" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="D14" s="4" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>R;;;Armor, +1;-;DMG(152)</v>
+        <v>R;Studded;N;Glamoured Studded Leather;-;DMG(172)</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>469</v>
@@ -8388,26 +8750,26 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>649</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>476</v>
+        <v>650</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>R;Shield;Y;Arrow-catching Shield;-;DMG(152)</v>
+        <v>U;Medium:Heavy;N;Adamantine Armor;Not Hide;DMG(150)</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>469</v>
@@ -8422,23 +8784,26 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>650</v>
+        <v>405</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>R;Chain_Shirt;;Elven Chain;-;DMG(168)</v>
+        <v>U;Any;N;Mariner's Armor;-;DMG(181)</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>469</v>
@@ -8453,23 +8818,26 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>652</v>
+        <v>649</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>476</v>
+        <v>650</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>306</v>
+        <v>322</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>R;Studded;;Glamoured Studded Leather;-;DMG(172)</v>
+        <v>U;Medium:Heavy;N;Mithral Armor;Not Hide;DMG(182)</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>469</v>
@@ -8484,26 +8852,26 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>649</v>
+        <v>405</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>336</v>
+        <v>279</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>R;Shield;Y;Shield of Missile Attraction;-;DMG(200)</v>
+        <v>V;Any;N;Armor, +2;-;DMG(152)</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>469</v>
@@ -8518,23 +8886,26 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>649</v>
+        <v>644</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>273</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>336</v>
+        <v>297</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>R;Shield;;Shield, +2;-;DMG(200)</v>
+        <v>V;Plate;Y;Demon Armor;-;DMG(165)</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>469</v>
@@ -8549,23 +8920,26 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>653</v>
+        <v>651</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>273</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>654</v>
+        <v>476</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>U;Medium:Heavy;;Adamantine Armor;Not Hide;DMG(150)</v>
+        <v>V;Scale_Mail;Y;Dragon Scale Mail;-;DMG(165)</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>469</v>
@@ -8580,21 +8954,26 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B21" s="3"/>
+        <v>268</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="D21" s="4" t="s">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>476</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>U;;;Mariner's Armor;-;DMG(181)</v>
+        <v>V;Plate;N;Dwarven Plate;-;DMG(167)</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>469</v>
@@ -8608,24 +8987,12 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>636</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>654</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>322</v>
-      </c>
+      <c r="B22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="10"/>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>U;Medium:Heavy;;Mithral Armor;Not Hide;DMG(182)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>469</v>
@@ -8639,24 +9006,12 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>637</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>335</v>
-      </c>
+      <c r="B23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="10"/>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>U;Shield;;Sentinel Shield;-;DMG(199)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J23" t="s">
         <v>469</v>
@@ -8670,24 +9025,12 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>638</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>336</v>
-      </c>
+      <c r="B24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="10"/>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>U;Shield;;Shield, +1;-;DMG(200)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J24" t="s">
         <v>469</v>
@@ -8701,27 +9044,12 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>639</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>276</v>
-      </c>
+      <c r="B25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="10"/>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>V;Shield;Y;Animated Shield;-;DMG(151)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J25" t="s">
         <v>469</v>
@@ -8735,22 +9063,12 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="B26" s="3"/>
-      <c r="D26" s="4" t="s">
-        <v>640</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>279</v>
-      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="10"/>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>V;;;Armor, +2;-;DMG(152)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J26" t="s">
         <v>469</v>
@@ -8764,27 +9082,12 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>641</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>297</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="10"/>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>V;Plate;Y;Demon Armor;-;DMG(165)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J27" t="s">
         <v>469</v>
@@ -8798,27 +9101,12 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>642</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>297</v>
-      </c>
+      <c r="B28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="10"/>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>V;Scale_Mail;Y;Dragon Scale Mail;-;DMG(165)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J28" t="s">
         <v>469</v>
@@ -8832,24 +9120,12 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>643</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>300</v>
-      </c>
+      <c r="B29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="10"/>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>V;Plate;;Dwarven Plate;-;DMG(167)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J29" t="s">
         <v>469</v>
@@ -8863,24 +9139,12 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>644</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>336</v>
-      </c>
+      <c r="B30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="10"/>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>V;Shield;;Shield, +3;-;DMG(200)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J30" t="s">
         <v>469</v>
@@ -8894,27 +9158,12 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>645</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>339</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="10"/>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>V;Shield;Y;Spellguard Shield;-;DMG(201)</v>
+        <v>;;;;;</v>
       </c>
       <c r="J31" t="s">
         <v>469</v>
@@ -9006,7 +9255,7 @@
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="D36" s="4" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E36" s="10"/>
       <c r="H36" t="str">
@@ -10997,6 +11246,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
+    <sortCondition ref="A2:A29"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -11006,8 +11258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6C3802-DBEB-4250-8D3F-2527012114E8}">
   <dimension ref="A1:L265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11052,7 +11304,10 @@
         <v>265</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>618</v>
@@ -11065,7 +11320,7 @@
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(A2,";",B2,";",C2,";",D2,";",E2,";",F2)</f>
-        <v>C;Shield;;Shield of Expression;-;XGE(139)</v>
+        <v>C;Shield;N;Shield of Expression;-;XGE(139)</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>467</v>
@@ -11083,7 +11338,10 @@
         <v>267</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>625</v>
@@ -11096,7 +11354,7 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">CONCATENATE(A3,";",B3,";",C3,";",D3,";",E3,";",F3)</f>
-        <v>R;Shield;;Pariah's Shield;-;GGR(180)</v>
+        <v>R;Shield;N;Pariah's Shield;-;GGR(180)</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>467</v>
@@ -11114,7 +11372,7 @@
         <v>267</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>273</v>
@@ -11148,7 +11406,7 @@
         <v>267</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>273</v>
@@ -11182,10 +11440,13 @@
         <v>267</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>476</v>
@@ -11195,7 +11456,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>R;Shield;;Shield, +2 in addition;-;DMG(200)</v>
+        <v>R;Shield;N;Shield, +2 in addition;-;DMG(200)</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>469</v>
@@ -11213,10 +11474,13 @@
         <v>266</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>476</v>
@@ -11226,7 +11490,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>U;Shield;;Sentinel Shield;-;DMG(199)</v>
+        <v>U;Shield;N;Sentinel Shield;-;DMG(199)</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>469</v>
@@ -11244,10 +11508,13 @@
         <v>266</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>476</v>
@@ -11257,7 +11524,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>U;Shield;;Shield, +1 in addition;-;DMG(200)</v>
+        <v>U;Shield;N;Shield, +1 in addition;-;DMG(200)</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>469</v>
@@ -11275,13 +11542,13 @@
         <v>268</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>273</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>476</v>
@@ -11309,10 +11576,13 @@
         <v>268</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>476</v>
@@ -11322,7 +11592,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>V;Shield;;Shield, +3 in addition;-;DMG(200)</v>
+        <v>V;Shield;N;Shield, +3 in addition;-;DMG(200)</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>570</v>
@@ -11340,13 +11610,13 @@
         <v>268</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>273</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>476</v>
@@ -11828,7 +12098,7 @@
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="D36" s="4" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E36" s="10"/>
       <c r="H36" t="str">
@@ -13822,6 +14092,865 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F31">
     <sortCondition ref="A2:A31"/>
   </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CC1091-4C38-4BFD-B191-CC2728BC3FB0}">
+  <dimension ref="A1:I265"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="77.140625" customWidth="1"/>
+    <col min="4" max="4" width="1.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="82.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>668</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>669</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>722</v>
+      </c>
+      <c r="C2" t="s">
+        <v>675</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE(A2,";",B2,";",C2)</f>
+        <v>10;Azurite;An opaque mottled deep blue gemstone</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>723</v>
+      </c>
+      <c r="C3" t="s">
+        <v>676</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E53" si="0">CONCATENATE(A3,";",B3,";",C3)</f>
+        <v>10;Banded Agate;A translucent striped brown, blue, white, or red gemstone</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>724</v>
+      </c>
+      <c r="C4" t="s">
+        <v>681</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Blue quartz;A transparent pale blue gemstone</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>725</v>
+      </c>
+      <c r="C5" t="s">
+        <v>692</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Eye agate;A translucent gemstone with circles of gray, white, brown, blue, or green</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>726</v>
+      </c>
+      <c r="C6" t="s">
+        <v>695</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Hematite;An opaque gray-black gemstone</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>727</v>
+      </c>
+      <c r="C7" t="s">
+        <v>700</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Lapis Lazuli;An opaque light and dark blue gemstone with yellow flecks</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>728</v>
+      </c>
+      <c r="C8" t="s">
+        <v>701</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Malachite;An opaque striated light and dark green gemstone</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>729</v>
+      </c>
+      <c r="C9" t="s">
+        <v>703</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Moss agate;A translucent gemstone with pink or yellow-white with mossy gray or green markings</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>730</v>
+      </c>
+      <c r="C10" t="s">
+        <v>704</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Obsidian;An opaque black gemstone</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>731</v>
+      </c>
+      <c r="C11" t="s">
+        <v>710</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Rhodochrosite;An opaque light pink gemstone</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>732</v>
+      </c>
+      <c r="C12" t="s">
+        <v>717</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Tiger Eye;A translucent brown gemstone with a golden center</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>733</v>
+      </c>
+      <c r="C13" t="s">
+        <v>720</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>10;Turquoise;An opaque light blue-green gemstone</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>734</v>
+      </c>
+      <c r="C14" t="s">
+        <v>680</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Bloodstone;An opaque dark gray gemstone with red flecks</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>735</v>
+      </c>
+      <c r="C15" t="s">
+        <v>684</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Carnelian;An opaque orange to red-brown gemstone</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>736</v>
+      </c>
+      <c r="C16" t="s">
+        <v>685</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Chalcedony;An opaque white gemstone</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>737</v>
+      </c>
+      <c r="C17" t="s">
+        <v>687</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Chrysoprase;A translucent green gemstone</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>738</v>
+      </c>
+      <c r="C18" t="s">
+        <v>688</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Citrine;A transparent pale yellow-brown gemstone</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>739</v>
+      </c>
+      <c r="C19" t="s">
+        <v>698</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Jasper;An opaque blue, black, or brown gemstone</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>740</v>
+      </c>
+      <c r="C20" t="s">
+        <v>702</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Moonstone;A translucent white gemstone with a pale blue glow</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>741</v>
+      </c>
+      <c r="C21" t="s">
+        <v>705</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Onyx;An opaque gemstone with bands of black and white, or pure black or white</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>742</v>
+      </c>
+      <c r="C22" t="s">
+        <v>709</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Quartz;A transparent white, smoky gray, or yellow gemstone</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>743</v>
+      </c>
+      <c r="C23" t="s">
+        <v>712</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Sardonyx;An opaque gemstone with bands of red and white</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>744</v>
+      </c>
+      <c r="C24" t="s">
+        <v>714</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Star Rose Quartz;A translucent rosy Gemstone with a white star-shaped center</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>745</v>
+      </c>
+      <c r="C25" t="s">
+        <v>673</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>50;Zircon;A transparent pale blue-green gemstone</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>746</v>
+      </c>
+      <c r="C26" t="s">
+        <v>674</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Amber;A transparent watery gold to rich gold gemstone</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <v>100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>747</v>
+      </c>
+      <c r="C27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Amethyst;A transparent deep purple gemstone</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>748</v>
+      </c>
+      <c r="C28" t="s">
+        <v>686</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Chrysoberyl;A transparent yellow-green to pale green gemstone</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>100</v>
+      </c>
+      <c r="B29" t="s">
+        <v>749</v>
+      </c>
+      <c r="C29" t="s">
+        <v>689</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Coral;An opaque crimson gemstone</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>750</v>
+      </c>
+      <c r="C30" t="s">
+        <v>694</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Garnet;A transparent red, brown-green, or violet gemstone</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>751</v>
+      </c>
+      <c r="C31" t="s">
+        <v>697</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Jade;A translucent light green, deep green, or white gemstone</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C32" t="s">
+        <v>699</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Jet;An opaque deep black gemstone</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <v>100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>753</v>
+      </c>
+      <c r="C33" t="s">
+        <v>707</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Pearl;An opaque lustrous white, yellow, or pink gemstone</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>754</v>
+      </c>
+      <c r="C34" t="s">
+        <v>713</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Spinel;A transparent gemstone of red, red-brown, or deep green</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
+        <v>755</v>
+      </c>
+      <c r="C35" t="s">
+        <v>719</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>100;Tourmaline;A transparent pale green, blue, brown, or red gemstone</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <v>500</v>
+      </c>
+      <c r="B36" t="s">
+        <v>756</v>
+      </c>
+      <c r="C36" t="s">
+        <v>671</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>500;Alexandrite;A transparent dark green gemstone</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>500</v>
+      </c>
+      <c r="B37" t="s">
+        <v>757</v>
+      </c>
+      <c r="C37" t="s">
+        <v>673</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>500;Aquamarine;A transparent pale blue-green gemstone</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
+        <v>500</v>
+      </c>
+      <c r="B38" t="s">
+        <v>758</v>
+      </c>
+      <c r="C38" t="s">
+        <v>678</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>500;Black Pearl;An opaque pure black gemstone</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>500</v>
+      </c>
+      <c r="B39" t="s">
+        <v>759</v>
+      </c>
+      <c r="C39" t="s">
+        <v>683</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>500;Blue spinel;A transparent deep blue gemstone</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>500</v>
+      </c>
+      <c r="B40" t="s">
+        <v>760</v>
+      </c>
+      <c r="C40" t="s">
+        <v>708</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>500;Peridot;A transparent rich olive green gemstone</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>500</v>
+      </c>
+      <c r="B41" t="s">
+        <v>761</v>
+      </c>
+      <c r="C41" t="s">
+        <v>718</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>500;Topaz;A transparent golden yellow gemstone</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B42" t="s">
+        <v>762</v>
+      </c>
+      <c r="C42" t="s">
+        <v>677</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>1000;Black Opal;A translucent dark green with black mottling and golden flecks gemstone</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B43" t="s">
+        <v>763</v>
+      </c>
+      <c r="C43" t="s">
+        <v>682</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>1000;Blue Sapphire;A transparent blue-white to medium blue gemstone</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B44" t="s">
+        <v>764</v>
+      </c>
+      <c r="C44" t="s">
+        <v>691</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>1000;Emerald;A transparent deep bright green gemstone</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B45" t="s">
+        <v>765</v>
+      </c>
+      <c r="C45" t="s">
+        <v>693</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>1000;Fire Opal;A translucent fiery red Gemstone</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B46" t="s">
+        <v>766</v>
+      </c>
+      <c r="C46" t="s">
+        <v>706</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>1000;Opal;A translucent pale blue with green and golden mottling gemstone</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B47" t="s">
+        <v>767</v>
+      </c>
+      <c r="C47" t="s">
+        <v>715</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>1000;Star Ruby;A translucent ruby gemstone with a white star-shaped center</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B48" t="s">
+        <v>768</v>
+      </c>
+      <c r="C48" t="s">
+        <v>716</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>1000;Star Sapphire;A translucent blue sapphire gemstone with a white star-shaped center</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="13">
+        <v>1000</v>
+      </c>
+      <c r="B49" t="s">
+        <v>769</v>
+      </c>
+      <c r="C49" t="s">
+        <v>721</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>1000;Yellow sapphire;A transparent fiery yellow or yellow-green gemstone</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="13">
+        <v>5000</v>
+      </c>
+      <c r="B50" t="s">
+        <v>770</v>
+      </c>
+      <c r="C50" t="s">
+        <v>679</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>5000;Black Sapphire;A translucent lustrous black gemstone with glowing highlights</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="13">
+        <v>5000</v>
+      </c>
+      <c r="B51" t="s">
+        <v>771</v>
+      </c>
+      <c r="C51" t="s">
+        <v>690</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="0"/>
+        <v>5000;Diamond;A transparent blue-white, canary, pink, brown, or blue gemstone</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="13">
+        <v>5000</v>
+      </c>
+      <c r="B52" t="s">
+        <v>772</v>
+      </c>
+      <c r="C52" t="s">
+        <v>696</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="0"/>
+        <v>5000;Jacinth;A transparent fiery orange gemstone</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>5000</v>
+      </c>
+      <c r="B53" t="s">
+        <v>773</v>
+      </c>
+      <c r="C53" t="s">
+        <v>711</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="0"/>
+        <v>5000;Ruby;A transparent clear red to deep crimson gemstone</v>
+      </c>
+    </row>
+    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E258" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E259" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="260" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E260" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="261" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E261" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="262" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E262" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="263" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E263" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="264" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E264" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="265" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E265" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>